<commit_message>
Rasha Comment _ Code Enhancements
</commit_message>
<xml_diff>
--- a/Sample.Automation.Solution.Tests/Data/TestData.xlsx
+++ b/Sample.Automation.Solution.Tests/Data/TestData.xlsx
@@ -85,18 +85,9 @@
     <t>33*2321</t>
   </si>
   <si>
-    <t>CreateNewUser2</t>
-  </si>
-  <si>
-    <t>CreateNewUser1</t>
-  </si>
-  <si>
     <t>Dina12s</t>
   </si>
   <si>
-    <t>ManagerLogin</t>
-  </si>
-  <si>
     <t>Data used by the manager to login the control page</t>
   </si>
   <si>
@@ -104,6 +95,15 @@
   </si>
   <si>
     <t>mgr!23</t>
+  </si>
+  <si>
+    <t>Create_New_User1</t>
+  </si>
+  <si>
+    <t>Create_New_User2</t>
+  </si>
+  <si>
+    <t>Manager_Login</t>
   </si>
 </sst>
 </file>
@@ -483,7 +483,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,7 +540,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>12</v>
@@ -579,7 +579,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>12</v>
@@ -610,7 +610,7 @@
         <v>987658374</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L3" t="s">
         <v>20</v>
@@ -658,16 +658,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>